<commit_message>
Added processed_by_mirth to all forms (Issue #2 )
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/baseline.xlsx
+++ b/xforms/xlsforms/baseline.xlsx
@@ -270,9 +270,6 @@
     <t>${dateOfBirth}&gt;${dateOfMigration} and ../migrationType = 'BASELINE'</t>
   </si>
   <si>
-    <t>${migrationType} = ''</t>
-  </si>
-  <si>
     <t>visit_date</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>processed</t>
+  </si>
+  <si>
+    <t>1=2</t>
   </si>
 </sst>
 </file>
@@ -1537,10 +1537,10 @@
   <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
+      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1680,10 +1680,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -1709,7 +1709,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>22</v>
@@ -1729,7 +1729,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>25</v>
@@ -1749,7 +1749,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
@@ -1798,7 +1798,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>30</v>
@@ -1821,7 +1821,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>32</v>
@@ -1844,7 +1844,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>34</v>
@@ -1861,10 +1861,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>35</v>
@@ -1885,7 +1885,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>37</v>
@@ -1931,7 +1931,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>42</v>
@@ -1991,16 +1991,16 @@
         <v>46</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>63</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I20" s="16" t="b">
         <v>1</v>
@@ -2017,7 +2017,7 @@
         <v>65</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I21" s="16" t="b">
         <v>1</v>
@@ -2044,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
@@ -2065,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2073,10 +2073,10 @@
         <v>40</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>80</v>
@@ -2085,7 +2085,7 @@
         <v>63</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I24" s="17" t="b">
         <v>1</v>
@@ -2102,10 +2102,10 @@
         <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2122,7 +2122,7 @@
         <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>71</v>
@@ -2136,19 +2136,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2311,7 +2311,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>50</v>
@@ -2325,7 +2325,7 @@
         <v>49</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>51</v>
@@ -2339,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>52</v>
@@ -2353,7 +2353,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>53</v>
@@ -2367,7 +2367,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>76</v>
@@ -2382,7 +2382,7 @@
         <v>74</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>75</v>
@@ -2678,7 +2678,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Naming conventions in baseline form
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/baseline.xlsx
+++ b/xforms/xlsforms/baseline.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-15" windowWidth="15600" windowHeight="11580" tabRatio="500"/>
+    <workbookView xWindow="25605" yWindow="-15" windowWidth="15600" windowHeight="11580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>type</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>select_one partialDate</t>
-  </si>
-  <si>
     <t>partialDate</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>Place member Moved FROM:</t>
   </si>
   <si>
-    <t>movedfrom</t>
-  </si>
-  <si>
     <t>select_one yes_no</t>
   </si>
   <si>
@@ -270,9 +264,6 @@
     <t>${dateOfBirth}&gt;${dateOfMigration} and ../migrationType = 'BASELINE'</t>
   </si>
   <si>
-    <t>visit_date</t>
-  </si>
-  <si>
     <t>Date of residency start</t>
   </si>
   <si>
@@ -351,9 +342,6 @@
     <t>baseline</t>
   </si>
   <si>
-    <t>middlename</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -364,6 +352,21 @@
   </si>
   <si>
     <t>1=2</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>movedFrom</t>
+  </si>
+  <si>
+    <t>visitDate</t>
+  </si>
+  <si>
+    <t>select_one partial_date</t>
+  </si>
+  <si>
+    <t>partial_date</t>
   </si>
 </sst>
 </file>
@@ -1536,11 +1539,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1567,13 +1570,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>18</v>
@@ -1657,7 +1660,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1680,10 +1683,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -1709,7 +1712,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>22</v>
@@ -1729,7 +1732,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>25</v>
@@ -1749,7 +1752,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
@@ -1763,13 +1766,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -1798,7 +1801,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>30</v>
@@ -1807,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M11" s="5" t="b">
         <v>1</v>
@@ -1821,7 +1824,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>32</v>
@@ -1830,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M12" s="5" t="b">
         <v>1</v>
@@ -1844,7 +1847,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>34</v>
@@ -1853,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1861,10 +1864,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>35</v>
@@ -1874,7 +1877,7 @@
       <c r="G14" s="2"/>
       <c r="I14" s="4"/>
       <c r="L14" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1885,7 +1888,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>37</v>
@@ -1897,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1920,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1931,7 +1934,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>42</v>
@@ -1939,27 +1942,27 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I17" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1968,12 +1971,12 @@
         <v>1</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1988,19 +1991,19 @@
         <v>40</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I20" s="16" t="b">
         <v>1</v>
@@ -2011,19 +2014,19 @@
     </row>
     <row r="21" spans="1:13" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>65</v>
-      </c>
       <c r="D21" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I21" s="16" t="b">
         <v>1</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2031,11 +2034,11 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2044,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
@@ -2052,11 +2055,11 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2065,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2073,19 +2076,19 @@
         <v>40</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I24" s="17" t="b">
         <v>1</v>
@@ -2096,16 +2099,16 @@
     </row>
     <row r="25" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2116,16 +2119,16 @@
     </row>
     <row r="26" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2136,19 +2139,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2276,8 +2279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2297,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>17</v>
@@ -2308,13 +2311,13 @@
         <v>39</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2322,70 +2325,70 @@
         <v>39</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="B5" s="12">
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="C7" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E7"/>
     </row>
@@ -2664,24 +2667,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaning of baseline form
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/baseline.xlsx
+++ b/xforms/xlsforms/baseline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-15" windowWidth="15600" windowHeight="11580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25605" yWindow="-15" windowWidth="15600" windowHeight="11580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
   <si>
     <t>type</t>
   </si>
@@ -156,9 +156,6 @@
     <t>dateOfMigration</t>
   </si>
   <si>
-    <t>reason</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>warning</t>
   </si>
   <si>
-    <t>Place member Moved FROM:</t>
-  </si>
-  <si>
     <t>select_one yes_no</t>
   </si>
   <si>
@@ -355,9 +349,6 @@
   </si>
   <si>
     <t>middleName</t>
-  </si>
-  <si>
-    <t>movedFrom</t>
   </si>
   <si>
     <t>visitDate</t>
@@ -1537,13 +1528,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1570,13 +1561,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>18</v>
@@ -1660,7 +1651,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1683,10 +1674,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -1712,7 +1703,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>22</v>
@@ -1732,7 +1723,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>25</v>
@@ -1752,7 +1743,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
@@ -1766,13 +1757,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -1801,7 +1792,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>30</v>
@@ -1810,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M11" s="5" t="b">
         <v>1</v>
@@ -1824,7 +1815,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>32</v>
@@ -1833,7 +1824,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M12" s="5" t="b">
         <v>1</v>
@@ -1847,7 +1838,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>34</v>
@@ -1856,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1864,10 +1855,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>35</v>
@@ -1877,7 +1868,7 @@
       <c r="G14" s="2"/>
       <c r="I14" s="4"/>
       <c r="L14" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1888,7 +1879,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>37</v>
@@ -1900,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1923,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1934,7 +1925,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>42</v>
@@ -1942,18 +1933,18 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I17" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>43</v>
@@ -1971,12 +1962,12 @@
         <v>1</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1994,16 +1985,16 @@
         <v>45</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D20" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="I20" s="16" t="b">
         <v>1</v>
@@ -2014,52 +2005,59 @@
     </row>
     <row r="21" spans="1:13" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="D21" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I21" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="I22" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="B23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2067,92 +2065,62 @@
       <c r="I23" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="11" t="s">
+    </row>
+    <row r="24" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I24" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="M24" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="I25" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="I24" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="I26" s="4" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>111</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
@@ -2162,6 +2130,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
@@ -2181,7 +2150,6 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -2193,33 +2161,20 @@
       <c r="G31" s="2"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I38" s="3"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I46" s="3"/>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I36" s="3"/>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="3"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I54" s="3"/>
@@ -2230,11 +2185,11 @@
     <row r="56" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I57" s="3"/>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I58" s="3"/>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I74" s="3"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I75" s="3"/>
@@ -2246,28 +2201,22 @@
       <c r="I77" s="3"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
       <c r="I78" s="3"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="3"/>
       <c r="I79" s="3"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="I80" s="3"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I81" s="3"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="3"/>
-      <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I83" s="3"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I85" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2279,7 +2228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2300,7 +2249,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>17</v>
@@ -2311,13 +2260,13 @@
         <v>39</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2325,70 +2274,70 @@
         <v>39</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B5" s="12">
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>72</v>
-      </c>
       <c r="C7" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E7"/>
     </row>
@@ -2667,24 +2616,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>